<commit_message>
Vagas mais arrumadas para GITHUB
</commit_message>
<xml_diff>
--- a/VAGASresee.xlsx
+++ b/VAGASresee.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DVH0\rearrange\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F0AA605-6038-4461-BBE8-77E4B963C052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13677F32-B6DF-4036-BCDA-05BB0DA55388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{FBD3203A-12B5-4F12-A2EC-6D55F28A17C7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Competência técnica</t>
   </si>
@@ -105,6 +105,120 @@
   </si>
   <si>
     <t>2) APRESENTAÇÃO RES</t>
+  </si>
+  <si>
+    <t>fel 2 fel3 ?</t>
+  </si>
+  <si>
+    <t>Exploração e desenvolvilmento</t>
+  </si>
+  <si>
+    <t>Curvas de produção</t>
+  </si>
+  <si>
+    <t>Produção</t>
+  </si>
+  <si>
+    <t>Planejamento e acompanhamento de dados</t>
+  </si>
+  <si>
+    <t>Gerenciamento de dados</t>
+  </si>
+  <si>
+    <t>Otimização da produção</t>
+  </si>
+  <si>
+    <t>Produtos finais</t>
+  </si>
+  <si>
+    <t>Modelos numéricos e definição de planos</t>
+  </si>
+  <si>
+    <t>Otimização do potencial do poço com atualização das previsões</t>
+  </si>
+  <si>
+    <t>Mantra</t>
+  </si>
+  <si>
+    <t>Modelo 3D do meio poroso</t>
+  </si>
+  <si>
+    <t>Inovação</t>
+  </si>
+  <si>
+    <t>OBS: A integração de dados é importante (GIT)</t>
+  </si>
+  <si>
+    <t>RES-CT (competência técnica)</t>
+  </si>
+  <si>
+    <t>Simulação</t>
+  </si>
+  <si>
+    <t>Avaliação de formação</t>
+  </si>
+  <si>
+    <t>Oportunidades e Projetos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulação </t>
+  </si>
+  <si>
+    <t>Projetos</t>
+  </si>
+  <si>
+    <t>Gerenciamento e Maximização do potencial</t>
+  </si>
+  <si>
+    <t>Gerenciamento</t>
+  </si>
+  <si>
+    <t>Focos</t>
+  </si>
+  <si>
+    <t>2 vagas simulação de reservatórios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 vaga Avaliação de formação: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interpreta inputs (ex: testes) </t>
+  </si>
+  <si>
+    <t>Apoia incorporação (filtrar inputs)</t>
+  </si>
+  <si>
+    <t>Lida com restrição de recurso (priorizar inpts)</t>
+  </si>
+  <si>
+    <t>Coordena outputs</t>
+  </si>
+  <si>
+    <t>Vantagens ----</t>
+  </si>
+  <si>
+    <t>Ebarque eventual</t>
+  </si>
+  <si>
+    <t>Plantão sobreaviso</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incentivo </t>
+  </si>
+  <si>
+    <t>Gosto por matemática</t>
+  </si>
+  <si>
+    <t>Modelagem de fluidos, interação rocha fluido</t>
+  </si>
+  <si>
+    <t>Construção modelos 3D</t>
+  </si>
+  <si>
+    <t>Implementa novas tecnologias</t>
+  </si>
+  <si>
+    <t>Coordena eventos técnicos disseminar conhecimento</t>
   </si>
 </sst>
 </file>
@@ -157,7 +271,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +296,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -354,10 +474,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -380,6 +501,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,8 +536,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>309637</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3967237</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
@@ -748,16 +877,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D97DA5E7-41A8-47E6-88D5-2343F8D77AE1}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -770,7 +899,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="22">
+      <c r="A4" s="23">
         <v>2</v>
       </c>
     </row>
@@ -805,86 +934,86 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:5" s="19" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:5" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
@@ -893,20 +1022,194 @@
       <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="4"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
       <c r="C23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="1:5" s="21" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="20" t="s">
+    <row r="25" spans="1:5" s="22" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="21" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C29" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C30" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="26"/>
+      <c r="B39" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="26"/>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="26"/>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="26"/>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B52" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A37:A38"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>